<commit_message>
Added mailing list member
</commit_message>
<xml_diff>
--- a/scBioinfoMailingList.xlsx
+++ b/scBioinfoMailingList.xlsx
@@ -298,7 +298,7 @@
     <t xml:space="preserve">anastasia.de-poulpiquet@curie.fr</t>
   </si>
   <si>
-    <t xml:space="preserve">melissa.saichi@inserm.fr</t>
+    <t xml:space="preserve">melissa.saichi@curie.fr</t>
   </si>
   <si>
     <t xml:space="preserve">remi.montagne@curie.fr</t>
@@ -632,8 +632,8 @@
   </sheetPr>
   <dimension ref="A1:A116"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A117" activeCellId="0" sqref="A117"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D98" activeCellId="0" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1101,7 +1101,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>92</v>
       </c>
@@ -1245,6 +1245,7 @@
     <hyperlink ref="A78" r:id="rId25" display="Victor.Renault@curie.fr"/>
     <hyperlink ref="A85" r:id="rId26" display="silvia.lopez-lastra@curie.fr"/>
     <hyperlink ref="A92" r:id="rId27" display="alexey.vorobev@curie.fr"/>
+    <hyperlink ref="A94" r:id="rId28" display="melissa.saichi@curie"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
added person mailing list
</commit_message>
<xml_diff>
--- a/scBioinfoMailingList.xlsx
+++ b/scBioinfoMailingList.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t xml:space="preserve">ScBioinfoMailingList</t>
   </si>
@@ -365,6 +365,9 @@
   </si>
   <si>
     <t xml:space="preserve">maxime.dubail@curie.fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yuna.landais@onebiosciences.fr</t>
   </si>
 </sst>
 </file>
@@ -554,13 +557,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -626,20 +629,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A116"/>
+  <dimension ref="A1:A117"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D98" activeCellId="0" sqref="D98"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A118" activeCellId="0" sqref="A118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.61"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1214,6 +1214,11 @@
     <row r="116" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1245,7 +1250,8 @@
     <hyperlink ref="A78" r:id="rId25" display="Victor.Renault@curie.fr"/>
     <hyperlink ref="A85" r:id="rId26" display="silvia.lopez-lastra@curie.fr"/>
     <hyperlink ref="A92" r:id="rId27" display="alexey.vorobev@curie.fr"/>
-    <hyperlink ref="A94" r:id="rId28" display="melissa.saichi@curie"/>
+    <hyperlink ref="A94" r:id="rId28" display="melissa.saichi@curie.fr"/>
+    <hyperlink ref="A117" r:id="rId29" display="yuna.landais@onebiosciences.fr"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>